<commit_message>
add cross companies and new version
</commit_message>
<xml_diff>
--- a/documentation/MathValidation.xlsx
+++ b/documentation/MathValidation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12100" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="1580" yWindow="0" windowWidth="25360" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="43">
   <si>
     <t>Vendor Identifier</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>16 Chain Calculation Intertable with sandwich SM2</t>
+  </si>
+  <si>
+    <t>Customer Two</t>
+  </si>
+  <si>
+    <t>New Data Version</t>
   </si>
 </sst>
 </file>
@@ -150,7 +156,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -316,7 +322,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -420,6 +426,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -504,9 +526,9 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="102" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="102" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="102" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="102" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="169">
     <cellStyle name="Comma" xfId="102" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -583,6 +605,14 @@
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -658,6 +688,14 @@
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
@@ -988,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1585,7 +1623,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:14">
       <c r="A33" s="11" t="s">
         <v>29</v>
       </c>
@@ -1594,7 +1632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:14">
       <c r="A34" s="11" t="s">
         <v>30</v>
       </c>
@@ -1603,7 +1641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:14">
       <c r="A35" s="11" t="s">
         <v>31</v>
       </c>
@@ -1612,7 +1650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:14">
       <c r="A36" s="11" t="s">
         <v>32</v>
       </c>
@@ -1621,7 +1659,7 @@
         <v>0.20960000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:14">
       <c r="A37" s="11" t="s">
         <v>33</v>
       </c>
@@ -1630,7 +1668,7 @@
         <v>0.41920000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:14">
       <c r="A38" s="11" t="s">
         <v>34</v>
       </c>
@@ -1639,7 +1677,7 @@
         <v>0.83840000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:14">
       <c r="A39" s="11" t="s">
         <v>35</v>
       </c>
@@ -1648,7 +1686,7 @@
         <v>4.1048</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:14">
       <c r="A40" s="11" t="s">
         <v>36</v>
       </c>
@@ -1657,7 +1695,7 @@
         <v>4.1048</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:14">
       <c r="A41" s="11" t="s">
         <v>37</v>
       </c>
@@ -1666,7 +1704,7 @@
         <v>4.1048</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:14">
       <c r="A42" s="11" t="s">
         <v>39</v>
       </c>
@@ -1675,7 +1713,7 @@
         <v>11.3712</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:14">
       <c r="A43" s="11" t="s">
         <v>38</v>
       </c>
@@ -1684,13 +1722,803 @@
         <v>0.9476</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:14">
       <c r="A44" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B44" s="31">
         <f>SUM(D26:D27)*SUM(N26:N27)</f>
         <v>7.5808</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J48" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K48" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L48" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M48" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N48" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <v>30</v>
+      </c>
+      <c r="D49">
+        <v>20</v>
+      </c>
+      <c r="E49" s="14">
+        <v>41791</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" s="15">
+        <f>C49*D49</f>
+        <v>600</v>
+      </c>
+      <c r="J49" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="K49" s="15">
+        <f>D49*J49</f>
+        <v>14</v>
+      </c>
+      <c r="L49" s="15">
+        <f>J49*I49</f>
+        <v>420</v>
+      </c>
+      <c r="M49" s="15">
+        <f>I49-L49</f>
+        <v>180</v>
+      </c>
+      <c r="N49" s="17">
+        <f>M49/I49</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50">
+        <v>30</v>
+      </c>
+      <c r="D50">
+        <v>20</v>
+      </c>
+      <c r="E50" s="14">
+        <v>41791</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="15">
+        <f>C50*D50</f>
+        <v>600</v>
+      </c>
+      <c r="J50" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="K50" s="15">
+        <f t="shared" ref="K50:K52" si="2">D50*J50</f>
+        <v>14</v>
+      </c>
+      <c r="L50" s="15">
+        <f>J50*I50</f>
+        <v>420</v>
+      </c>
+      <c r="M50" s="15">
+        <f>I50-L50</f>
+        <v>180</v>
+      </c>
+      <c r="N50" s="17">
+        <f>M50/I50</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51">
+        <v>30</v>
+      </c>
+      <c r="D51">
+        <v>20</v>
+      </c>
+      <c r="E51" s="14">
+        <v>41791</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I51" s="15">
+        <f>C51*D51</f>
+        <v>600</v>
+      </c>
+      <c r="J51" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="K51" s="15">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="L51" s="15">
+        <f>J51*I51</f>
+        <v>420</v>
+      </c>
+      <c r="M51" s="15">
+        <f>I51-L51</f>
+        <v>180</v>
+      </c>
+      <c r="N51" s="17">
+        <f>M51/I51</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>30</v>
+      </c>
+      <c r="D52">
+        <v>20</v>
+      </c>
+      <c r="E52" s="21">
+        <v>41791</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" s="22">
+        <f>C52*D52</f>
+        <v>600</v>
+      </c>
+      <c r="J52" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="K52" s="22">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="L52" s="22">
+        <f>J52*I52</f>
+        <v>420</v>
+      </c>
+      <c r="M52" s="22">
+        <f>I52-L52</f>
+        <v>180</v>
+      </c>
+      <c r="N52" s="24">
+        <f>M52/I52</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53" s="2"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="27">
+        <f>SUM(C49:C52)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="28">
+        <f>SUM(I49:I52)</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="29">
+        <f>(SUM(C49:C50)*SUM(D49:D50))+(C51*D51)+ (C52*D52)</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" s="29">
+        <f>SUM(C49:C52)*SUM(D49:D52)</f>
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="29">
+        <f>(SUM(C49:D49)+SUM(C50:D50)+SUM(C51:D51)+SUM(C52:D52))</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="29">
+        <f>(SUM(C49:C50)+SUM(D49:D50))+SUM(C51:D51)+SUM(C52:D52)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="29">
+        <f>SUM(C49:C52)+SUM(D49:D52)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="29">
+        <f>SUM(K49:K52)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" s="29">
+        <f>SUM(D49:D50)*SUM(J49:J50)+(D51*J51)+(D52+J52)</f>
+        <v>90.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B63" s="29">
+        <f>SUM(D49:D52)*SUM(K49:K52)</f>
+        <v>4480</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" s="29">
+        <f>(D49+J49)+(D50+J50)+(D51+J51)+(D52+J52)</f>
+        <v>82.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" s="29">
+        <f>SUM(D49:D50)+SUM(J49:J50)+D51+J51+D52+J52</f>
+        <v>82.8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66" s="29">
+        <f>SUM(D49:D52)+SUM(J49:J52)</f>
+        <v>82.8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" s="32">
+        <f>SUM(M49:M52)</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" s="32">
+        <f>SUM(M49:M52)/SUM(I49:I52)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B69" s="30">
+        <f>SUM(D49:D52)*SUM(N49:N52)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J73" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K73" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L73" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M73" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N73" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="13">
+        <v>300</v>
+      </c>
+      <c r="D74" s="13">
+        <v>200</v>
+      </c>
+      <c r="E74" s="14">
+        <v>41791</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I74" s="15">
+        <f>C74*D74</f>
+        <v>60000</v>
+      </c>
+      <c r="J74" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="K74" s="15">
+        <f>D74*J74</f>
+        <v>140</v>
+      </c>
+      <c r="L74" s="15">
+        <f>J74*I74</f>
+        <v>42000</v>
+      </c>
+      <c r="M74" s="15">
+        <f>I74-L74</f>
+        <v>18000</v>
+      </c>
+      <c r="N74" s="17">
+        <f>M74/I74</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" s="13">
+        <v>0</v>
+      </c>
+      <c r="D75" s="13">
+        <v>0</v>
+      </c>
+      <c r="E75" s="14">
+        <v>41791</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H75" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I75" s="15">
+        <f>C75*D75</f>
+        <v>0</v>
+      </c>
+      <c r="J75" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="K75" s="15">
+        <f t="shared" ref="K75:K77" si="3">D75*J75</f>
+        <v>0</v>
+      </c>
+      <c r="L75" s="15">
+        <f>J75*I75</f>
+        <v>0</v>
+      </c>
+      <c r="M75" s="15">
+        <f>I75-L75</f>
+        <v>0</v>
+      </c>
+      <c r="N75" s="17" t="e">
+        <f>M75/I75</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="13">
+        <v>0</v>
+      </c>
+      <c r="D76" s="13">
+        <v>0</v>
+      </c>
+      <c r="E76" s="14">
+        <v>41791</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H76" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I76" s="15">
+        <f>C76*D76</f>
+        <v>0</v>
+      </c>
+      <c r="J76" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="K76" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L76" s="15">
+        <f>J76*I76</f>
+        <v>0</v>
+      </c>
+      <c r="M76" s="15">
+        <f>I76-L76</f>
+        <v>0</v>
+      </c>
+      <c r="N76" s="17" t="e">
+        <f>M76/I76</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="20">
+        <v>3</v>
+      </c>
+      <c r="D77" s="20">
+        <v>2</v>
+      </c>
+      <c r="E77" s="21">
+        <v>41791</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G77" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I77" s="22">
+        <f>C77*D77</f>
+        <v>6</v>
+      </c>
+      <c r="J77" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="K77" s="22">
+        <f t="shared" si="3"/>
+        <v>1.4</v>
+      </c>
+      <c r="L77" s="22">
+        <f>J77*I77</f>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="M77" s="22">
+        <f>I77-L77</f>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="N77" s="24">
+        <f>M77/I77</f>
+        <v>0.3000000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="E78" s="2"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="4"/>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="A79" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" s="27">
+        <f>SUM(C74:C77)</f>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="A80" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" s="28">
+        <f>SUM(I74:I77)</f>
+        <v>60006</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B81" s="29">
+        <f>(SUM(C74:C75)*SUM(D74:D75))+(C76*D76)+ (C77*D77)</f>
+        <v>60006</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B82" s="29">
+        <f>SUM(C74:C77)*SUM(D74:D77)</f>
+        <v>61206</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B83" s="29">
+        <f>(SUM(C74:D74)+SUM(C75:D75)+SUM(C76:D76)+SUM(C77:D77))</f>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B84" s="29">
+        <f>(SUM(C74:C75)+SUM(D74:D75))+SUM(C76:D76)+SUM(C77:D77)</f>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85" s="29">
+        <f>SUM(C74:C77)+SUM(D74:D77)</f>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" s="29">
+        <f>SUM(K74:K77)</f>
+        <v>141.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B87" s="29">
+        <f>SUM(D74:D75)*SUM(J74:J75)+(D76*J76)+(D77+J77)</f>
+        <v>282.7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B88" s="29">
+        <f>SUM(D74:D77)*SUM(K74:K77)</f>
+        <v>28562.800000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" s="29">
+        <f>(D74+J74)+(D75+J75)+(D76+J76)+(D77+J77)</f>
+        <v>204.79999999999995</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B90" s="29">
+        <f>SUM(D74:D75)+SUM(J74:J75)+D76+J76+D77+J77</f>
+        <v>204.79999999999998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B91" s="29">
+        <f>SUM(D74:D77)+SUM(J74:J77)</f>
+        <v>204.8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B92" s="32">
+        <f>SUM(M74:M77)</f>
+        <v>18001.8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B93" s="32">
+        <f>SUM(M74:M77)/SUM(I74:I77)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B94" s="30" t="e">
+        <f>SUM(D74:D77)*SUM(N74:N77)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix Math Validation formula error
</commit_message>
<xml_diff>
--- a/documentation/MathValidation.xlsx
+++ b/documentation/MathValidation.xlsx
@@ -322,7 +322,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="169">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -426,6 +426,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -528,7 +532,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="102" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="102" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="169">
+  <cellStyles count="173">
     <cellStyle name="Comma" xfId="102" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -613,6 +617,8 @@
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -696,6 +702,8 @@
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
@@ -1028,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="N75" sqref="N75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1373,8 +1381,8 @@
         <v>33</v>
       </c>
       <c r="B15" s="29">
-        <f>SUM(D2:D3)*SUM(J2:J3)+(D4*J4)+(D5+J5)</f>
-        <v>2.8239999999999998</v>
+        <f>SUM(D2:D3)*SUM(J2:J3)+(D4*J4)+(D5*J5)</f>
+        <v>0.82880000000000009</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -2060,8 +2068,8 @@
         <v>33</v>
       </c>
       <c r="B62" s="29">
-        <f>SUM(D49:D50)*SUM(J49:J50)+(D51*J51)+(D52+J52)</f>
-        <v>90.7</v>
+        <f>SUM(D49:D50)*SUM(J49:J50)+(D51*J51)+(D52*J52)</f>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -2454,8 +2462,8 @@
         <v>33</v>
       </c>
       <c r="B87" s="29">
-        <f>SUM(D74:D75)*SUM(J74:J75)+(D76*J76)+(D77+J77)</f>
-        <v>282.7</v>
+        <f>SUM(D74:D75)*SUM(J74:J75)+(D76*J76)+(D77*J77)</f>
+        <v>281.39999999999998</v>
       </c>
     </row>
     <row r="88" spans="1:2">

</xml_diff>

<commit_message>
added docs for quarterly aggregation test verification
</commit_message>
<xml_diff>
--- a/documentation/MathValidation.xlsx
+++ b/documentation/MathValidation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="0" windowWidth="25360" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="1200" yWindow="0" windowWidth="25360" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="48">
   <si>
     <t>Vendor Identifier</t>
   </si>
@@ -148,6 +148,21 @@
   </si>
   <si>
     <t>New Data Version</t>
+  </si>
+  <si>
+    <t>Filter Scenario</t>
+  </si>
+  <si>
+    <t>Date Range Quarter 2 = 2014/04/01 : 2014/06/30</t>
+  </si>
+  <si>
+    <t>* Notice that date variable, now refers to the QUARTER PERIOD</t>
+  </si>
+  <si>
+    <t>3 Case Multiplication, with groupby (Vendor Identifier, Product Type Idenfier,date)</t>
+  </si>
+  <si>
+    <t>Quarterly Aggregation Scenario</t>
   </si>
 </sst>
 </file>
@@ -164,7 +179,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -213,7 +227,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +246,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -321,6 +359,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -497,7 +550,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -531,6 +584,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="102" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="102" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="5" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="6" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="5" xfId="102" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="173">
     <cellStyle name="Comma" xfId="102" builtinId="3"/>
@@ -1034,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O94"/>
+  <dimension ref="A1:O123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="N75" sqref="N75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1448,6 +1521,11 @@
         <v>29.523199999999999</v>
       </c>
     </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="25" spans="1:14">
       <c r="A25" s="6" t="s">
         <v>0</v>
@@ -2528,6 +2606,769 @@
         <f>SUM(D74:D77)*SUM(N74:N77)</f>
         <v>#DIV/0!</v>
       </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" s="12" customFormat="1">
+      <c r="A97" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E97" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F97" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G97" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H97" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="I97" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="J97" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="K97" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="L97" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="M97" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="N97" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" s="37" customFormat="1">
+      <c r="A98" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="34">
+        <v>3</v>
+      </c>
+      <c r="D98" s="34">
+        <v>2</v>
+      </c>
+      <c r="E98" s="35">
+        <v>41730</v>
+      </c>
+      <c r="F98" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H98" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I98" s="34">
+        <f>C98*D98</f>
+        <v>6</v>
+      </c>
+      <c r="J98" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="K98" s="34">
+        <f>D98*J98</f>
+        <v>0.4</v>
+      </c>
+      <c r="L98" s="34">
+        <f>J98*I98</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="M98" s="34">
+        <f>I98-L98</f>
+        <v>4.8</v>
+      </c>
+      <c r="N98" s="34">
+        <f>M98/I98</f>
+        <v>0.79999999999999993</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" s="41" customFormat="1">
+      <c r="A99" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B99" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="38">
+        <v>3</v>
+      </c>
+      <c r="D99" s="38">
+        <v>2</v>
+      </c>
+      <c r="E99" s="39">
+        <v>41791</v>
+      </c>
+      <c r="F99" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="H99" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="I99" s="38">
+        <f t="shared" ref="I99:I105" si="4">C99*D99</f>
+        <v>6</v>
+      </c>
+      <c r="J99" s="40">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="K99" s="38">
+        <f>D99*J99</f>
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="L99" s="38">
+        <f>J99*I99</f>
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="M99" s="38">
+        <f t="shared" ref="M99:M105" si="5">I99-L99</f>
+        <v>5.9711999999999996</v>
+      </c>
+      <c r="N99" s="38">
+        <f t="shared" ref="N99:N104" si="6">M99/I99</f>
+        <v>0.99519999999999997</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" s="41" customFormat="1">
+      <c r="A100" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="38">
+        <v>3</v>
+      </c>
+      <c r="D100" s="38">
+        <v>2</v>
+      </c>
+      <c r="E100" s="39">
+        <v>41791</v>
+      </c>
+      <c r="F100" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H100" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I100" s="38">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="J100" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="K100" s="38">
+        <f t="shared" ref="K100:K105" si="7">D100*J100</f>
+        <v>0.2</v>
+      </c>
+      <c r="L100" s="38">
+        <f>J100*I100</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="M100" s="38">
+        <f t="shared" si="5"/>
+        <v>5.4</v>
+      </c>
+      <c r="N100" s="38">
+        <f t="shared" si="6"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" s="37" customFormat="1">
+      <c r="A101" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B101" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="34">
+        <v>3</v>
+      </c>
+      <c r="D101" s="34">
+        <v>2</v>
+      </c>
+      <c r="E101" s="35">
+        <v>41791</v>
+      </c>
+      <c r="F101" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G101" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I101" s="34">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="J101" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="K101" s="34">
+        <f t="shared" si="7"/>
+        <v>0.4</v>
+      </c>
+      <c r="L101" s="34">
+        <f>J101*I101</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="M101" s="34">
+        <f t="shared" si="5"/>
+        <v>4.8</v>
+      </c>
+      <c r="N101" s="34">
+        <f t="shared" si="6"/>
+        <v>0.79999999999999993</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" s="46" customFormat="1">
+      <c r="A102" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" s="43">
+        <v>3</v>
+      </c>
+      <c r="D102" s="43">
+        <v>2</v>
+      </c>
+      <c r="E102" s="44">
+        <v>41791</v>
+      </c>
+      <c r="F102" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G102" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="H102" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I102" s="43">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="J102" s="45">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="K102" s="43">
+        <f>D102*J102</f>
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="L102" s="43">
+        <f>J102*I102</f>
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="M102" s="43">
+        <f t="shared" si="5"/>
+        <v>5.9711999999999996</v>
+      </c>
+      <c r="N102" s="43">
+        <f t="shared" si="6"/>
+        <v>0.99519999999999997</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" s="41" customFormat="1">
+      <c r="A103" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B103" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="38">
+        <v>4</v>
+      </c>
+      <c r="D103" s="38">
+        <v>3</v>
+      </c>
+      <c r="E103" s="39">
+        <v>41792</v>
+      </c>
+      <c r="F103" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H103" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I103" s="38">
+        <f>C103*D103</f>
+        <v>12</v>
+      </c>
+      <c r="J103" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="K103" s="38">
+        <f t="shared" si="7"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="L103" s="38">
+        <f t="shared" ref="L103:L105" si="8">J103*I103</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="M103" s="38">
+        <f t="shared" si="5"/>
+        <v>10.8</v>
+      </c>
+      <c r="N103" s="38">
+        <f t="shared" si="6"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" s="12" customFormat="1">
+      <c r="A104" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104" s="33">
+        <v>4</v>
+      </c>
+      <c r="D104" s="33">
+        <v>3</v>
+      </c>
+      <c r="E104" s="47">
+        <v>41883</v>
+      </c>
+      <c r="F104" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="G104" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H104" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I104" s="33">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="J104" s="48">
+        <v>0.1</v>
+      </c>
+      <c r="K104" s="33">
+        <f t="shared" si="7"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="L104" s="33">
+        <f t="shared" si="8"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="M104" s="33">
+        <f t="shared" si="5"/>
+        <v>10.8</v>
+      </c>
+      <c r="N104" s="33">
+        <f t="shared" si="6"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" s="12" customFormat="1">
+      <c r="A105" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="33">
+        <v>4</v>
+      </c>
+      <c r="D105" s="33">
+        <v>3</v>
+      </c>
+      <c r="E105" s="47">
+        <v>41977</v>
+      </c>
+      <c r="F105" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="G105" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H105" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I105" s="33">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="J105" s="48">
+        <v>0.1</v>
+      </c>
+      <c r="K105" s="33">
+        <f t="shared" si="7"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="L105" s="33">
+        <f t="shared" si="8"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="M105" s="33">
+        <f t="shared" si="5"/>
+        <v>10.8</v>
+      </c>
+      <c r="N105" s="33">
+        <f>M105/I105</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15">
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="2"/>
+      <c r="H106" s="12"/>
+      <c r="I106" s="12"/>
+      <c r="J106" s="49"/>
+      <c r="K106" s="12"/>
+      <c r="L106" s="12"/>
+      <c r="M106" s="12"/>
+      <c r="N106" s="12"/>
+      <c r="O106" s="1"/>
+    </row>
+    <row r="107" spans="1:15">
+      <c r="A107" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B107" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="12"/>
+      <c r="G107" s="12"/>
+      <c r="H107" s="12"/>
+      <c r="I107" s="12"/>
+      <c r="J107" s="51"/>
+      <c r="K107" s="12"/>
+      <c r="L107" s="12"/>
+      <c r="M107" s="12"/>
+      <c r="N107" s="12"/>
+      <c r="O107" s="1"/>
+    </row>
+    <row r="108" spans="1:15">
+      <c r="A108" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B108" s="27">
+        <f>SUM(C98:C103)</f>
+        <v>19</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1"/>
+    </row>
+    <row r="109" spans="1:15">
+      <c r="A109" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B109" s="52">
+        <f>SUM(I98:I103)</f>
+        <v>42</v>
+      </c>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1"/>
+    </row>
+    <row r="110" spans="1:15">
+      <c r="A110" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B110" s="29">
+        <f>((C98+C101)*(D98+D101))+((C99+C100+C103)*(D99+D100+D103))+(C102*D102)</f>
+        <v>100</v>
+      </c>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1"/>
+    </row>
+    <row r="111" spans="1:15">
+      <c r="A111" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B111" s="29">
+        <f>SUM(C98:C103)*SUM(D98:D103)</f>
+        <v>247</v>
+      </c>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+      <c r="O111" s="1"/>
+    </row>
+    <row r="112" spans="1:15">
+      <c r="A112" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B112" s="29">
+        <f>(SUM(C98:D98)+SUM(C99:D99)+SUM(C100:D100)+SUM(C101:D101)+SUM(C102:D102)+SUM(C103:D103))</f>
+        <v>32</v>
+      </c>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+      <c r="O112" s="1"/>
+    </row>
+    <row r="113" spans="1:15">
+      <c r="A113" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B113" s="29">
+        <f>((C98+C101)+(D98+D101))+((C99+C100+C103)+(D99+D100+D103))+(C102+D102)</f>
+        <v>32</v>
+      </c>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1"/>
+    </row>
+    <row r="114" spans="1:15">
+      <c r="A114" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B114" s="29">
+        <f>SUM(C98:C103)+SUM(D98:D103)</f>
+        <v>32</v>
+      </c>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+      <c r="O114" s="1"/>
+    </row>
+    <row r="115" spans="1:15">
+      <c r="A115" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B115" s="29">
+        <f>SUM(K98:K103)</f>
+        <v>1.3192000000000002</v>
+      </c>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="L115" s="1"/>
+      <c r="M115" s="1"/>
+      <c r="N115" s="1"/>
+      <c r="O115" s="1"/>
+    </row>
+    <row r="116" spans="1:15">
+      <c r="A116" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B116" s="29">
+        <f>((D98+D101)*(J98+J101))+((D99+D100+D103)*(J99+J100+J103))+(D102*J102)</f>
+        <v>3.0431999999999997</v>
+      </c>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
+      <c r="J116" s="1"/>
+      <c r="L116" s="1"/>
+      <c r="M116" s="1"/>
+      <c r="N116" s="1"/>
+      <c r="O116" s="1"/>
+    </row>
+    <row r="117" spans="1:15">
+      <c r="A117" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B117" s="29">
+        <f>SUM(D98:D103)*SUM(K98:K103)</f>
+        <v>17.149600000000003</v>
+      </c>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="L117" s="1"/>
+      <c r="M117" s="1"/>
+      <c r="N117" s="1"/>
+      <c r="O117" s="1"/>
+    </row>
+    <row r="118" spans="1:15">
+      <c r="A118" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B118" s="29">
+        <f>(D98+J98)+(D99+J99)+(D100+J100)+(D101+J101)+D102+J102+D103+J103</f>
+        <v>13.609599999999999</v>
+      </c>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+      <c r="L118" s="1"/>
+      <c r="M118" s="1"/>
+      <c r="N118" s="1"/>
+      <c r="O118" s="1"/>
+    </row>
+    <row r="119" spans="1:15">
+      <c r="A119" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B119" s="29">
+        <f>((D98+D101)+(J98+J101))+((D99+D100+D103)+(J99+J100+J103))+(D102+J102)</f>
+        <v>13.6096</v>
+      </c>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="L119" s="1"/>
+      <c r="M119" s="1"/>
+      <c r="N119" s="1"/>
+      <c r="O119" s="1"/>
+    </row>
+    <row r="120" spans="1:15">
+      <c r="A120" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B120" s="29">
+        <f>SUM(D98:D103)+SUM(J98:J103)</f>
+        <v>13.6096</v>
+      </c>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="L120" s="1"/>
+      <c r="M120" s="1"/>
+      <c r="N120" s="1"/>
+      <c r="O120" s="1"/>
+    </row>
+    <row r="121" spans="1:15">
+      <c r="A121" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B121" s="32">
+        <f>SUM(M98:M103)</f>
+        <v>37.742400000000004</v>
+      </c>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+      <c r="J121" s="1"/>
+      <c r="L121" s="1"/>
+      <c r="M121" s="1"/>
+      <c r="N121" s="1"/>
+      <c r="O121" s="1"/>
+    </row>
+    <row r="122" spans="1:15">
+      <c r="A122" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B122" s="32">
+        <f>SUM(M98:M103)/SUM(I98:I103)</f>
+        <v>0.89862857142857155</v>
+      </c>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="L122" s="1"/>
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
+      <c r="O122" s="1"/>
+    </row>
+    <row r="123" spans="1:15">
+      <c r="A123" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B123" s="30">
+        <f>SUM(D98:D103)*SUM(N98:N103)</f>
+        <v>70.075199999999995</v>
+      </c>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1"/>
+      <c r="L123" s="1"/>
+      <c r="M123" s="1"/>
+      <c r="N123" s="1"/>
+      <c r="O123" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>